<commit_message>
commit problems with the model
</commit_message>
<xml_diff>
--- a/outputs/DeliveryStartTime.xlsx
+++ b/outputs/DeliveryStartTime.xlsx
@@ -340,24 +340,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:X6"/>
+  <dimension ref="A1:H6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:24">
+    <row r="1" spans="1:8">
       <c r="A1">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B1">
-        <v>10</v>
+        <v>9964</v>
       </c>
       <c r="C1">
-        <v>19954.00000000777</v>
+        <v>10</v>
       </c>
       <c r="D1">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E1">
         <v>10</v>
@@ -366,288 +366,96 @@
         <v>10</v>
       </c>
       <c r="G1">
-        <v>19954.00000000608</v>
+        <v>0</v>
       </c>
       <c r="H1">
-        <v>19954.00000000579</v>
-      </c>
-      <c r="I1">
-        <v>19954.00000000509</v>
-      </c>
-      <c r="J1">
-        <v>9998.000000000004</v>
-      </c>
-      <c r="K1">
-        <v>19954.00000000402</v>
-      </c>
-      <c r="L1">
-        <v>19954.00000000357</v>
-      </c>
-      <c r="M1">
-        <v>19954.00000000309</v>
-      </c>
-      <c r="N1">
-        <v>19954.0000000026</v>
-      </c>
-      <c r="O1">
-        <v>19954.00000000227</v>
-      </c>
-      <c r="P1">
-        <v>0</v>
-      </c>
-      <c r="Q1">
-        <v>19954.00000000175</v>
-      </c>
-      <c r="R1">
-        <v>19954.00000000141</v>
-      </c>
-      <c r="S1">
-        <v>0</v>
-      </c>
-      <c r="T1">
-        <v>0</v>
-      </c>
-      <c r="U1">
-        <v>0</v>
-      </c>
-      <c r="V1">
-        <v>0</v>
-      </c>
-      <c r="W1">
-        <v>0</v>
-      </c>
-      <c r="X1">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:24">
+    <row r="2" spans="1:8">
       <c r="A2">
-        <v>9954</v>
+        <v>10</v>
       </c>
       <c r="B2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>9954</v>
+        <v>10</v>
       </c>
       <c r="D2">
-        <v>9958</v>
+        <v>10000</v>
       </c>
       <c r="E2">
-        <v>19954.0000000007</v>
+        <v>10</v>
       </c>
       <c r="F2">
-        <v>0</v>
+        <v>10010</v>
       </c>
       <c r="G2">
-        <v>0</v>
+        <v>9964</v>
       </c>
       <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>19954.00000000486</v>
-      </c>
-      <c r="J2">
-        <v>19954.00000000425</v>
-      </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
-      <c r="L2">
-        <v>0</v>
-      </c>
-      <c r="M2">
-        <v>0</v>
-      </c>
-      <c r="N2">
-        <v>0</v>
-      </c>
-      <c r="O2">
-        <v>0</v>
-      </c>
-      <c r="P2">
-        <v>0</v>
-      </c>
-      <c r="Q2">
-        <v>19954.0000000016</v>
-      </c>
-      <c r="R2">
-        <v>19954.0000000014</v>
-      </c>
-      <c r="S2">
-        <v>19954.00000000116</v>
-      </c>
-      <c r="T2">
-        <v>19954.00000000083</v>
-      </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>0</v>
-      </c>
-      <c r="W2">
-        <v>0</v>
-      </c>
-      <c r="X2">
-        <v>0</v>
+        <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="1:24">
+    <row r="3" spans="1:8">
       <c r="A3">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B3">
-        <v>19954.00000000594</v>
+        <v>10</v>
       </c>
       <c r="C3">
-        <v>19954.0000000057</v>
+        <v>9969</v>
       </c>
       <c r="D3">
-        <v>19954.00000000547</v>
+        <v>30</v>
       </c>
       <c r="E3">
-        <v>19954.00000000489</v>
+        <v>0</v>
       </c>
       <c r="F3">
-        <v>19954.00000000463</v>
+        <v>0</v>
       </c>
       <c r="G3">
-        <v>19954.00000000422</v>
+        <v>0</v>
       </c>
       <c r="H3">
-        <v>19954.00000000365</v>
-      </c>
-      <c r="I3">
-        <v>19954.00000000293</v>
-      </c>
-      <c r="J3">
-        <v>19954.00000000257</v>
-      </c>
-      <c r="K3">
-        <v>0</v>
-      </c>
-      <c r="L3">
-        <v>0</v>
-      </c>
-      <c r="M3">
-        <v>0</v>
-      </c>
-      <c r="N3">
-        <v>0</v>
-      </c>
-      <c r="O3">
-        <v>0</v>
-      </c>
-      <c r="P3">
-        <v>19954.00000000084</v>
-      </c>
-      <c r="Q3">
-        <v>19954.00000000068</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3">
-        <v>0</v>
-      </c>
-      <c r="T3">
-        <v>0</v>
-      </c>
-      <c r="U3">
-        <v>19954.00000000031</v>
-      </c>
-      <c r="V3">
-        <v>19954.00000000031</v>
-      </c>
-      <c r="W3">
-        <v>19954.00000000031</v>
-      </c>
-      <c r="X3">
-        <v>19954.00000000031</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24">
+    <row r="4" spans="1:8">
       <c r="A4">
-        <v>9957</v>
+        <v>10</v>
       </c>
       <c r="B4">
-        <v>7034.000000000004</v>
+        <v>0</v>
       </c>
       <c r="C4">
         <v>10</v>
       </c>
       <c r="D4">
-        <v>10</v>
+        <v>10000</v>
       </c>
       <c r="E4">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="F4">
-        <v>19954.00000000083</v>
+        <v>0</v>
       </c>
       <c r="G4">
-        <v>19954.00000000069</v>
+        <v>0</v>
       </c>
       <c r="H4">
-        <v>19954.00000000045</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4">
-        <v>0</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="L4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>19954.00000000329</v>
-      </c>
-      <c r="N4">
-        <v>19954.00000000276</v>
-      </c>
-      <c r="O4">
-        <v>19954.00000000247</v>
-      </c>
-      <c r="P4">
-        <v>19954.00000000217</v>
-      </c>
-      <c r="Q4">
-        <v>0</v>
-      </c>
-      <c r="R4">
-        <v>0</v>
-      </c>
-      <c r="S4">
-        <v>0</v>
-      </c>
-      <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4">
-        <v>0</v>
-      </c>
-      <c r="V4">
-        <v>0</v>
-      </c>
-      <c r="W4">
-        <v>0</v>
-      </c>
-      <c r="X4">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:24">
+    <row r="5" spans="1:8">
       <c r="A5">
-        <v>9957</v>
+        <v>10</v>
       </c>
       <c r="B5">
-        <v>7783.000000000004</v>
+        <v>10</v>
       </c>
       <c r="C5">
         <v>10</v>
@@ -659,135 +467,39 @@
         <v>10</v>
       </c>
       <c r="F5">
-        <v>10</v>
+        <v>10000</v>
       </c>
       <c r="G5">
-        <v>10</v>
+        <v>19964</v>
       </c>
       <c r="H5">
-        <v>19954.00000000057</v>
-      </c>
-      <c r="I5">
-        <v>0</v>
-      </c>
-      <c r="J5">
-        <v>0</v>
-      </c>
-      <c r="K5">
-        <v>0</v>
-      </c>
-      <c r="L5">
-        <v>0</v>
-      </c>
-      <c r="M5">
-        <v>0</v>
-      </c>
-      <c r="N5">
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <v>0</v>
-      </c>
-      <c r="P5">
-        <v>0</v>
-      </c>
-      <c r="Q5">
-        <v>0</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
-      </c>
-      <c r="S5">
-        <v>0</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5">
-        <v>0</v>
-      </c>
-      <c r="V5">
-        <v>0</v>
-      </c>
-      <c r="W5">
-        <v>0</v>
-      </c>
-      <c r="X5">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:24">
+    <row r="6" spans="1:8">
       <c r="A6">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="B6">
-        <v>9998.000000000004</v>
+        <v>10</v>
       </c>
       <c r="C6">
-        <v>19954.00000000711</v>
+        <v>9964</v>
       </c>
       <c r="D6">
-        <v>9990</v>
+        <v>9979</v>
       </c>
       <c r="E6">
-        <v>7783.000000000004</v>
+        <v>9965</v>
       </c>
       <c r="F6">
-        <v>19954.00000000533</v>
+        <v>10000</v>
       </c>
       <c r="G6">
-        <v>19954.00000000474</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>19954.00000000409</v>
-      </c>
-      <c r="I6">
-        <v>9998.000000000004</v>
-      </c>
-      <c r="J6">
-        <v>19954.00000000294</v>
-      </c>
-      <c r="K6">
-        <v>10</v>
-      </c>
-      <c r="L6">
-        <v>19954.00000000224</v>
-      </c>
-      <c r="M6">
-        <v>19954.00000000193</v>
-      </c>
-      <c r="N6">
-        <v>10</v>
-      </c>
-      <c r="O6">
-        <v>19954.00000000136</v>
-      </c>
-      <c r="P6">
-        <v>19954.00000000105</v>
-      </c>
-      <c r="Q6">
-        <v>9998.000000000004</v>
-      </c>
-      <c r="R6">
-        <v>19954.00000000057</v>
-      </c>
-      <c r="S6">
-        <v>0</v>
-      </c>
-      <c r="T6">
-        <v>19954.00000000028</v>
-      </c>
-      <c r="U6">
-        <v>19954.00000000067</v>
-      </c>
-      <c r="V6">
-        <v>10</v>
-      </c>
-      <c r="W6">
-        <v>19954.00000000043</v>
-      </c>
-      <c r="X6">
-        <v>19954.00000000021</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>